<commit_message>
Add extended menutree source file, which was missing in previous commit.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -1194,8 +1194,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2674,7 +2674,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="50" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="50" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;K000000&amp;F</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added callback function for validating forms (before persisting the data to the database). Unit test completed.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21660" yWindow="0" windowWidth="25605" windowHeight="15660" tabRatio="500"/>
+    <workbookView xWindow="21660" yWindow="0" windowWidth="25605" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="help" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$G$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$H$53</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="259">
   <si>
     <t>Liste mit allen FahrerInnen</t>
   </si>
@@ -705,6 +705,123 @@
   </si>
   <si>
     <t>ANONYM</t>
+  </si>
+  <si>
+    <t>BREADCRUMB</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Disposition - Produktionsplan</t>
+  </si>
+  <si>
+    <t>Disposition - Monatsplan</t>
+  </si>
+  <si>
+    <t>Disposition - Tagesplan</t>
+  </si>
+  <si>
+    <t>Disposition - Fahrauftrag</t>
+  </si>
+  <si>
+    <t>Disposition - Fahrwegoptimierung</t>
+  </si>
+  <si>
+    <t>Fahrgast - Fahrgastliste</t>
+  </si>
+  <si>
+    <t>Fahrgast - Fahrgastdaten</t>
+  </si>
+  <si>
+    <t>Fahrgast - Dauerauftrag</t>
+  </si>
+  <si>
+    <t>Fahrgast - Abwesenheit</t>
+  </si>
+  <si>
+    <t>Fahrgast - Details</t>
+  </si>
+  <si>
+    <t>Fahrgast - Anrufmaske</t>
+  </si>
+  <si>
+    <t>OVI - OVI-Liste</t>
+  </si>
+  <si>
+    <t>OVI - OVI-Daten</t>
+  </si>
+  <si>
+    <t>Fahrer - Fahrerliste</t>
+  </si>
+  <si>
+    <t>Fahrer - Fahrerdaten</t>
+  </si>
+  <si>
+    <t>Fahrer - Wochenplan</t>
+  </si>
+  <si>
+    <t>Fahrer - Ferienplan</t>
+  </si>
+  <si>
+    <t>Fahrer - Einsatzplan</t>
+  </si>
+  <si>
+    <t>Fahrer - Details</t>
+  </si>
+  <si>
+    <t>Fahrer - Anrufmaske</t>
+  </si>
+  <si>
+    <t>Fahrzeug - Fahrzeugliste</t>
+  </si>
+  <si>
+    <t>Fahrzeug - Fahrzeugdaten</t>
+  </si>
+  <si>
+    <t>Fahrzeug - Serviceplan</t>
+  </si>
+  <si>
+    <t>Fahrzeug - Details</t>
+  </si>
+  <si>
+    <t>Bereitstellen - Fahrauftrag</t>
+  </si>
+  <si>
+    <t>Bereitstellen - Einsatzplaene</t>
+  </si>
+  <si>
+    <t>Bereitstellen - Fahreinsaetze</t>
+  </si>
+  <si>
+    <t>Bereitstellen - Monatsrechnung</t>
+  </si>
+  <si>
+    <t>Unterhalt - Organisationsdaten</t>
+  </si>
+  <si>
+    <t>Unterhalt - Teamdaten</t>
+  </si>
+  <si>
+    <t>Unterhalt - Logs</t>
+  </si>
+  <si>
+    <t>Unterhalt - Datenbank</t>
+  </si>
+  <si>
+    <t>Unterhalt - Feiertage</t>
+  </si>
+  <si>
+    <t>Unterhalt - Datenbank - Backup</t>
+  </si>
+  <si>
+    <t>Unterhalt - Datenbank - Aufraemen</t>
+  </si>
+  <si>
+    <t>Bereitstellen - Fahrauftrag - Mails</t>
+  </si>
+  <si>
+    <t>Bereitstellen - Fahrauftrag - Drucken</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1309,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1206,12 +1323,13 @@
     <col min="4" max="4" width="9" style="12" customWidth="1"/>
     <col min="5" max="5" width="33.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="66.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="1"/>
+    <col min="7" max="7" width="33.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="66.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>182</v>
       </c>
@@ -1231,13 +1349,16 @@
         <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1257,13 +1378,16 @@
         <v>184</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f>A2+1</f>
         <v>2</v>
@@ -1284,13 +1408,16 @@
         <v>187</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" ref="A4:A53" si="0">A3+1</f>
         <v>3</v>
@@ -1311,13 +1438,16 @@
         <v>189</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1338,13 +1468,16 @@
         <v>193</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1365,13 +1498,16 @@
         <v>192</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1392,13 +1528,16 @@
         <v>195</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1419,13 +1558,16 @@
         <v>199</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1446,13 +1588,16 @@
         <v>197</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1473,13 +1618,16 @@
         <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1500,13 +1648,16 @@
         <v>53</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1527,13 +1678,16 @@
         <v>54</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1554,13 +1708,16 @@
         <v>55</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1581,13 +1738,16 @@
         <v>56</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1608,13 +1768,16 @@
         <v>19</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1635,13 +1798,16 @@
         <v>29</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1662,13 +1828,16 @@
         <v>31</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1689,13 +1858,16 @@
         <v>32</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1716,13 +1888,16 @@
         <v>57</v>
       </c>
       <c r="G19" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1743,13 +1918,16 @@
         <v>58</v>
       </c>
       <c r="G20" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1770,13 +1948,16 @@
         <v>59</v>
       </c>
       <c r="G21" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1797,13 +1978,16 @@
         <v>60</v>
       </c>
       <c r="G22" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1824,13 +2008,16 @@
         <v>25</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1851,13 +2038,16 @@
         <v>12</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1878,13 +2068,16 @@
         <v>14</v>
       </c>
       <c r="G25" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1905,13 +2098,16 @@
         <v>26</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1932,13 +2128,16 @@
         <v>33</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1959,13 +2158,16 @@
         <v>1</v>
       </c>
       <c r="G28" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1986,13 +2188,16 @@
         <v>61</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2013,13 +2218,16 @@
         <v>62</v>
       </c>
       <c r="G30" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2040,13 +2248,16 @@
         <v>63</v>
       </c>
       <c r="G31" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2067,13 +2278,16 @@
         <v>59</v>
       </c>
       <c r="G32" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2094,13 +2308,16 @@
         <v>60</v>
       </c>
       <c r="G33" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2121,13 +2338,16 @@
         <v>27</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2148,13 +2368,16 @@
         <v>5</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2175,13 +2398,16 @@
         <v>7</v>
       </c>
       <c r="G36" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2202,13 +2428,16 @@
         <v>64</v>
       </c>
       <c r="G37" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2229,13 +2458,16 @@
         <v>59</v>
       </c>
       <c r="G38" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2256,13 +2488,16 @@
         <v>20</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2282,14 +2517,17 @@
       <c r="F40" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2309,14 +2547,17 @@
       <c r="F41" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="H41" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2336,14 +2577,17 @@
       <c r="F42" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2364,13 +2608,16 @@
         <v>66</v>
       </c>
       <c r="G43" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2391,13 +2638,16 @@
         <v>67</v>
       </c>
       <c r="G44" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2418,13 +2668,16 @@
         <v>68</v>
       </c>
       <c r="G45" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2444,14 +2697,17 @@
       <c r="F46" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2471,14 +2727,17 @@
       <c r="F47" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G47" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H47" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2499,13 +2758,16 @@
         <v>70</v>
       </c>
       <c r="G48" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2526,13 +2788,16 @@
         <v>71</v>
       </c>
       <c r="G49" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2552,14 +2817,17 @@
       <c r="F50" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="G50" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2580,13 +2848,16 @@
         <v>72</v>
       </c>
       <c r="G51" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2607,13 +2878,16 @@
         <v>73</v>
       </c>
       <c r="G52" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="H52" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2634,14 +2908,17 @@
         <v>74</v>
       </c>
       <c r="G53" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H53" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:G53"/>
+  <autoFilter ref="E1:H53"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="D2">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
Update menutree for vehicle data, details, serviceplan (enabled).
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -48,7 +48,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-must be the same as in  routing.yml</t>
+must be the same as the pattern in  routing.yml</t>
         </r>
       </text>
     </comment>
@@ -1316,8 +1316,8 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished Unit Test for the AutoForm, FormStateBuilder and ListBuilder services successfully.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -11,7 +11,7 @@
     <sheet name="help" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$46</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -57,13 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="245">
-  <si>
-    <t>Fahrerdaten</t>
-  </si>
-  <si>
-    <t>Daten vom FahrerIn</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="224">
   <si>
     <t xml:space="preserve">Vertrauliche Daten zu Fahrer </t>
   </si>
@@ -71,9 +65,6 @@
     <t>Angestossen wenn Fahrer die Zentrale anruft (Anruf Kennung)</t>
   </si>
   <si>
-    <t>Fahrzeugdaten</t>
-  </si>
-  <si>
     <t>Daten des Fahrzeuges</t>
   </si>
   <si>
@@ -86,12 +77,6 @@
     <t>Angestossen wenn Fahrgast die Zentrale anruft (Anruf Kennung)</t>
   </si>
   <si>
-    <t>OVI-Daten</t>
-  </si>
-  <si>
-    <t>Daten von einem Ort von Interesse</t>
-  </si>
-  <si>
     <t>Disposition</t>
   </si>
   <si>
@@ -137,9 +122,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>Fahrgastdaten</t>
-  </si>
-  <si>
     <t>Benutzerdaten definieren; Anmeldename, Passwort, Rolle</t>
   </si>
   <si>
@@ -150,9 +132,6 @@
   </si>
   <si>
     <t>Fahrauftrag pro Fahrer (Fahrzeug) und pro Schicht (optimiert)</t>
-  </si>
-  <si>
-    <t>Daten von den Fahrgaeste</t>
   </si>
   <si>
     <t>Wiederholende Fahrauftraege.</t>
@@ -324,9 +303,6 @@
     <t>/app/ovi</t>
   </si>
   <si>
-    <t>/app/ovi/daten</t>
-  </si>
-  <si>
     <t>/app/fahrer</t>
   </si>
   <si>
@@ -444,9 +420,6 @@
     <t>tixi_ovi_page</t>
   </si>
   <si>
-    <t>tixi_ovi_daten_page</t>
-  </si>
-  <si>
     <t>tixi_fahrer_page</t>
   </si>
   <si>
@@ -522,18 +495,6 @@
     <t>Splash Page Disposition</t>
   </si>
   <si>
-    <t>Splash Page Fahrgast</t>
-  </si>
-  <si>
-    <t>Splash Page Orte von Interesse (OVI)</t>
-  </si>
-  <si>
-    <t>Splash Page Fahrer</t>
-  </si>
-  <si>
-    <t>Splash Page Fahrzeug</t>
-  </si>
-  <si>
     <t>Splash Page Fahrauftrag</t>
   </si>
   <si>
@@ -690,9 +651,6 @@
     <t>Disposition - Fahrwegoptimierung</t>
   </si>
   <si>
-    <t>Fahrgast - Fahrgastdaten</t>
-  </si>
-  <si>
     <t>Fahrgast - Dauerauftrag</t>
   </si>
   <si>
@@ -705,12 +663,6 @@
     <t>Fahrgast - Anrufmaske</t>
   </si>
   <si>
-    <t>OVI - OVI-Daten</t>
-  </si>
-  <si>
-    <t>Fahrer - Fahrerdaten</t>
-  </si>
-  <si>
     <t>Fahrer - Wochenplan</t>
   </si>
   <si>
@@ -726,9 +678,6 @@
     <t>Fahrer - Anrufmaske</t>
   </si>
   <si>
-    <t>Fahrzeug - Fahrzeugdaten</t>
-  </si>
-  <si>
     <t>Fahrzeug - Serviceplan</t>
   </si>
   <si>
@@ -780,33 +729,12 @@
     <t>/app/ovi/details</t>
   </si>
   <si>
-    <t>OVI-Details</t>
-  </si>
-  <si>
     <t>OVI - OVI-Details</t>
   </si>
   <si>
     <t>Vertrauliche Daten zu OVI</t>
   </si>
   <si>
-    <t>tixi_fahrgast_daten_page</t>
-  </si>
-  <si>
-    <t>/app/fahrgast/daten</t>
-  </si>
-  <si>
-    <t>/app/fahrer/daten</t>
-  </si>
-  <si>
-    <t>tixi_fahrer_daten_page</t>
-  </si>
-  <si>
-    <t>/app/fahrzeug/daten</t>
-  </si>
-  <si>
-    <t>tixi_fahrzeug_daten_page</t>
-  </si>
-  <si>
     <t>tixi_unterhalt_teamdaten_page</t>
   </si>
   <si>
@@ -814,6 +742,15 @@
   </si>
   <si>
     <t>Unterhalt - Teamdaten</t>
+  </si>
+  <si>
+    <t>Fahrgast Daten</t>
+  </si>
+  <si>
+    <t>Orte von Interesse (OVI) Daten</t>
+  </si>
+  <si>
+    <t>Fahrer Daten</t>
   </si>
 </sst>
 </file>
@@ -1314,10 +1251,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1262,7 @@
     <col min="1" max="1" width="7.875" style="12" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="12" customWidth="1"/>
     <col min="3" max="3" width="37" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="12" customWidth="1"/>
     <col min="6" max="6" width="33.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.625" style="1" customWidth="1"/>
@@ -1337,34 +1274,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1372,28 +1309,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1402,58 +1339,58 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f t="shared" ref="A4:A50" si="0">A3+1</f>
+        <f t="shared" ref="A4:A46" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1462,28 +1399,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1492,28 +1429,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E6" s="12">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1522,28 +1459,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="E7" s="12">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1552,28 +1489,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E8" s="12">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1582,28 +1519,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="E9" s="12">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1612,28 +1549,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E10" s="12">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1642,28 +1579,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="12">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="I11" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1672,28 +1609,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E12" s="12">
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1702,28 +1639,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E13" s="12">
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1732,28 +1669,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E14" s="12">
         <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1762,28 +1699,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E15" s="12">
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1792,28 +1729,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E16" s="12">
         <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1822,94 +1759,97 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>236</v>
+        <v>110</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E18" s="12">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="J19" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1918,31 +1858,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>236</v>
+        <v>107</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1951,31 +1891,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>236</v>
+        <v>112</v>
       </c>
       <c r="E21" s="12">
         <v>0</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1984,28 +1921,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>120</v>
+        <v>214</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="E22" s="12">
         <v>0</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>80</v>
+      <c r="F22" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>148</v>
+        <v>44</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2014,28 +1954,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E23" s="12">
         <v>0</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2044,31 +1984,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>231</v>
+        <v>117</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E24" s="12">
         <v>0</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>232</v>
+      <c r="F24" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>233</v>
+        <v>44</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2077,28 +2017,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="E25" s="12">
         <v>0</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>82</v>
+      <c r="F25" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>149</v>
+        <v>46</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2107,28 +2050,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>239</v>
+        <v>115</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="E26" s="12">
         <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>238</v>
+        <v>76</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2137,31 +2083,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>239</v>
+        <v>113</v>
       </c>
       <c r="E27" s="12">
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2170,31 +2116,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>239</v>
+        <v>113</v>
       </c>
       <c r="E28" s="12">
         <v>0</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2203,31 +2149,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="E29" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>211</v>
+        <v>17</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2236,31 +2179,31 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="E30" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2269,31 +2212,31 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="E31" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2302,28 +2245,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E32" s="12">
         <v>0</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2332,28 +2275,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>241</v>
+        <v>123</v>
       </c>
       <c r="E33" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>240</v>
+        <v>84</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>5</v>
+        <v>201</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2362,31 +2305,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>241</v>
+        <v>124</v>
       </c>
       <c r="E34" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>51</v>
+        <v>85</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>6</v>
+        <v>211</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2395,31 +2335,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>241</v>
+        <v>125</v>
       </c>
       <c r="E35" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>56</v>
+        <v>86</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>36</v>
+        <v>212</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2428,28 +2365,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E36" s="12">
         <v>0</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>152</v>
+        <v>51</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2458,28 +2395,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E37" s="12">
         <v>0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>151</v>
+        <v>203</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2488,28 +2425,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E38" s="12">
         <v>0</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>67</v>
+        <v>89</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>37</v>
+        <v>204</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2518,28 +2455,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E39" s="12">
         <v>0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>57</v>
+        <v>90</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>38</v>
+        <v>11</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2548,28 +2485,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E40" s="12">
         <v>0</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>155</v>
+        <v>205</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2578,28 +2515,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>136</v>
+        <v>218</v>
       </c>
       <c r="E41" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>220</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>154</v>
+        <v>21</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2608,28 +2545,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E42" s="12">
         <v>0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2638,28 +2575,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E43" s="12">
         <v>0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2668,28 +2605,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E44" s="12">
         <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>157</v>
+        <v>209</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2698,28 +2635,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>242</v>
+        <v>134</v>
       </c>
       <c r="E45" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>243</v>
+        <v>95</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2728,154 +2665,34 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E46" s="12">
         <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="12">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E47" s="12">
-        <v>0</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="12">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E48" s="12">
-        <v>0</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="12">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" s="12">
-        <v>0</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="12">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="12">
-        <v>0</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I50"/>
+  <autoFilter ref="F1:I46"/>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E50">
+  <conditionalFormatting sqref="E2:E46">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2911,7 +2728,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2922,7 +2739,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2933,7 +2750,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2944,7 +2761,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>

</xml_diff>

<commit_message>
Added MysqlDumpBundle for the backup of customer databases on the server. Unit test completed successfully.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -1253,8 +1253,8 @@
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2611,7 +2611,7 @@
         <v>133</v>
       </c>
       <c r="E44" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Migrated to iTixi database schema v2, romoved MATCH ... AGAINST fulltext filters, these don't work, rolled back to where like ... Upgraded validation for serviceplan. Unit test completed, no issues.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -11,7 +11,7 @@
     <sheet name="help" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$45</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="226">
   <si>
     <t xml:space="preserve">Vertrauliche Daten zu Fahrer </t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Daten des Fahrzeuges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertrauliche Daten zu Fahrzeug </t>
   </si>
   <si>
     <t>Vertrauliche Daten zu Fahrgast</t>
@@ -327,9 +324,6 @@
     <t>/app/fahrzeug/serviceplan</t>
   </si>
   <si>
-    <t>/app/fahrzeug/details</t>
-  </si>
-  <si>
     <t>/app/bereitsellen</t>
   </si>
   <si>
@@ -444,9 +438,6 @@
     <t>tixi_fahrzeug_serviceplan_page</t>
   </si>
   <si>
-    <t>tixi_fahrzeug_details_page</t>
-  </si>
-  <si>
     <t>tixi_bereitsellen_page</t>
   </si>
   <si>
@@ -681,9 +672,6 @@
     <t>Fahrzeug - Serviceplan</t>
   </si>
   <si>
-    <t>Fahrzeug - Details</t>
-  </si>
-  <si>
     <t>Bereitstellen - Fahrauftrag</t>
   </si>
   <si>
@@ -751,6 +739,24 @@
   </si>
   <si>
     <t>Fahrer Daten</t>
+  </si>
+  <si>
+    <t>tixi_unterhalt_zonenplan_page</t>
+  </si>
+  <si>
+    <t>/app/unterhalt/zonenplan</t>
+  </si>
+  <si>
+    <t>Zonenplan</t>
+  </si>
+  <si>
+    <t>Unterhalt - Zonenplan</t>
+  </si>
+  <si>
+    <t>Splash Page Datenbank</t>
+  </si>
+  <si>
+    <t>Zonenplan für den Lieferschein einrichten</t>
   </si>
 </sst>
 </file>
@@ -1253,8 +1259,8 @@
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1274,34 +1280,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1309,28 +1315,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1339,28 +1345,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1369,28 +1375,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1399,28 +1405,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1429,28 +1435,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E6" s="12">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1459,28 +1465,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E7" s="12">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1489,28 +1495,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E8" s="12">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1519,28 +1525,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E9" s="12">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1549,28 +1555,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="12">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1579,28 +1585,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1609,28 +1615,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" s="12">
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1639,28 +1645,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E13" s="12">
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1669,28 +1675,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E14" s="12">
         <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1699,28 +1705,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E15" s="12">
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1729,28 +1735,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E16" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1759,31 +1765,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E17" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1792,31 +1798,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="12">
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1825,31 +1831,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E19" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1858,31 +1864,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1891,28 +1897,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E21" s="12">
         <v>0</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1921,31 +1927,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E22" s="12">
         <v>0</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1954,28 +1960,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E23" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1984,31 +1990,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E24" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2017,31 +2023,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E25" s="12">
         <v>0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2050,31 +2056,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E26" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2083,31 +2089,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E27" s="12">
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2116,31 +2122,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E28" s="12">
         <v>0</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2149,28 +2155,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E29" s="12">
         <v>1</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2179,31 +2185,31 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E30" s="12">
         <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2212,31 +2218,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E31" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2245,28 +2248,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E32" s="12">
         <v>0</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2275,28 +2278,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E33" s="12">
         <v>0</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>41</v>
+        <v>83</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>138</v>
+        <v>207</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2305,28 +2308,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E34" s="12">
         <v>0</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2335,28 +2338,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E35" s="12">
         <v>0</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>31</v>
+        <v>198</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2365,28 +2368,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E36" s="12">
         <v>0</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>51</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2395,28 +2398,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E37" s="12">
         <v>0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2425,28 +2428,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E38" s="12">
         <v>0</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="I38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>140</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2455,28 +2458,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E39" s="12">
         <v>0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>143</v>
+        <v>201</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2485,28 +2488,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="E40" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>91</v>
+        <v>215</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>144</v>
+        <v>216</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2515,28 +2518,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="E41" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>219</v>
+        <v>90</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2545,28 +2548,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E42" s="12">
         <v>0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>35</v>
+        <v>203</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2575,28 +2578,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E43" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>143</v>
+        <v>205</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2605,28 +2608,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E44" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2635,28 +2638,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E45" s="12">
         <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>58</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2665,35 +2668,45 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>135</v>
+        <v>220</v>
       </c>
       <c r="E46" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>96</v>
+        <v>221</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>59</v>
+        <v>222</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>12</v>
+        <v>225</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I46"/>
+  <autoFilter ref="F1:I45"/>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E46">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="E2:E45">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <color rgb="FF9BF183"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2728,7 +2741,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2739,7 +2752,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2750,7 +2763,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2761,7 +2774,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>

</xml_diff>

<commit_message>
Removed FahrzeugDetailsBundle, added OviDatenBundle and OviDetailsBundle. Fixed FormStateBuilder.setForeignKey. Unit test completed successfully.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -717,9 +717,6 @@
     <t>/app/ovi/details</t>
   </si>
   <si>
-    <t>OVI - OVI-Details</t>
-  </si>
-  <si>
     <t>Vertrauliche Daten zu OVI</t>
   </si>
   <si>
@@ -757,6 +754,9 @@
   </si>
   <si>
     <t>Zonenplan für den Lieferschein einrichten</t>
+  </si>
+  <si>
+    <t>OVI - Details</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1753,7 @@
         <v>18</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>97</v>
@@ -1903,7 +1903,7 @@
         <v>110</v>
       </c>
       <c r="E21" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>72</v>
@@ -1915,7 +1915,7 @@
         <v>14</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>97</v>
@@ -1936,7 +1936,7 @@
         <v>110</v>
       </c>
       <c r="E22" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>211</v>
@@ -1945,10 +1945,10 @@
         <v>43</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>213</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>98</v>
@@ -1978,7 +1978,7 @@
         <v>15</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>97</v>
@@ -2491,19 +2491,19 @@
         <v>169</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E40" s="12">
         <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>20</v>
@@ -2566,7 +2566,7 @@
         <v>203</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>98</v>
@@ -2671,22 +2671,22 @@
         <v>169</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E46" s="12">
         <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="H46" s="4" t="s">
-        <v>223</v>
-      </c>
       <c r="I46" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Added PassengerDataBundle, PassengerDetailsBundle, PassengerAbsenceBundle, ZoneplenBundle, HolidayBundle. One issue: display of foreign keys in list should be suppressed.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -1259,8 +1259,8 @@
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1738,22 +1738,22 @@
         <v>169</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E16" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>216</v>
+        <v>136</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>97</v>
@@ -1768,31 +1768,28 @@
         <v>169</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E17" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>3</v>
+        <v>197</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1801,25 +1798,22 @@
         <v>169</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="E18" s="12">
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>41</v>
+        <v>83</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>24</v>
+        <v>207</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>97</v>
@@ -1834,25 +1828,22 @@
         <v>169</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="E19" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>42</v>
+        <v>84</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>25</v>
+        <v>208</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>97</v>
@@ -1867,25 +1858,22 @@
         <v>169</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>97</v>
@@ -1900,22 +1888,22 @@
         <v>169</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="E21" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>217</v>
+        <v>51</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>97</v>
@@ -1930,25 +1918,22 @@
         <v>169</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="E22" s="12">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>211</v>
+        <v>0</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>212</v>
+        <v>137</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>98</v>
@@ -1963,22 +1948,22 @@
         <v>169</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E23" s="12">
         <v>1</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>73</v>
+      <c r="F23" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>97</v>
@@ -1993,31 +1978,31 @@
         <v>169</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E24" s="12">
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2026,25 +2011,25 @@
         <v>169</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E25" s="12">
         <v>0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>97</v>
@@ -2059,25 +2044,25 @@
         <v>169</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E26" s="12">
         <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>97</v>
@@ -2092,25 +2077,25 @@
         <v>169</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E27" s="12">
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>97</v>
@@ -2125,25 +2110,22 @@
         <v>169</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>97</v>
@@ -2158,25 +2140,28 @@
         <v>169</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>117</v>
+        <v>210</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="E29" s="12">
         <v>1</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>79</v>
+      <c r="F29" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2188,25 +2173,22 @@
         <v>169</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E30" s="12">
         <v>1</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>80</v>
+      <c r="F30" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>97</v>
@@ -2221,25 +2203,28 @@
         <v>169</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="J31" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2251,22 +2236,25 @@
         <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E32" s="12">
         <v>0</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>135</v>
+        <v>191</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>97</v>
@@ -2281,22 +2269,25 @@
         <v>169</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E33" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>59</v>
+        <v>75</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>29</v>
+        <v>192</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>97</v>
@@ -2311,22 +2302,25 @@
         <v>169</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E34" s="12">
         <v>0</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>49</v>
+        <v>76</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>30</v>
+        <v>193</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>97</v>
@@ -2341,22 +2335,25 @@
         <v>169</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E35" s="12">
         <v>0</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>139</v>
+        <v>1</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>97</v>
@@ -2371,22 +2368,22 @@
         <v>169</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E36" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>199</v>
+        <v>16</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>138</v>
+        <v>2</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>97</v>
@@ -2401,25 +2398,28 @@
         <v>169</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="E37" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2644,7 +2644,7 @@
         <v>132</v>
       </c>
       <c r="E45" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Added ShiftBundle for defining beginning and end of a working shift. Unit test completed.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="231">
   <si>
     <t xml:space="preserve">Vertrauliche Daten zu Fahrer </t>
   </si>
@@ -757,6 +757,21 @@
   </si>
   <si>
     <t>OVI - Details</t>
+  </si>
+  <si>
+    <t>tixi_unterhalt_dienste_page</t>
+  </si>
+  <si>
+    <t>/app/unterhalt/dienste</t>
+  </si>
+  <si>
+    <t>Dienste</t>
+  </si>
+  <si>
+    <t>Unterhalt - Dienste</t>
+  </si>
+  <si>
+    <t>Dienst Zeiten (Anfang - Ende) einrichten</t>
   </si>
 </sst>
 </file>
@@ -1257,10 +1272,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1386,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f t="shared" ref="A4:A46" si="0">A3+1</f>
+        <f t="shared" ref="A4:A47" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2671,24 +2686,54 @@
         <v>169</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E46" s="12">
         <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E47" s="12">
+        <v>1</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2696,7 +2741,17 @@
   <autoFilter ref="F1:I45"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="E2:E45">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <color rgb="FF9BF183"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>

</xml_diff>

<commit_message>
Permissions are mapped to each web page. Added check the page permission against the rules assigned to each user. Unit test successfull. Please note: the menutree database needs to be reimported.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -1274,8 +1274,8 @@
   </sheetPr>
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1289,7 @@
     <col min="7" max="7" width="19.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="33.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="66.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.75" style="1" customWidth="1"/>
     <col min="11" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
@@ -1951,7 +1951,7 @@
         <v>137</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>3</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2674,7 +2674,7 @@
         <v>11</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed OVI details, Fahrgast details, Fahrer datails, added Fahrzeug details bundle, fixed empty date defaults (jquery exception). Unit test successfull.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -11,7 +11,7 @@
     <sheet name="help" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$46</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="235">
   <si>
     <t xml:space="preserve">Vertrauliche Daten zu Fahrer </t>
   </si>
@@ -772,6 +772,18 @@
   </si>
   <si>
     <t>Dienst Zeiten (Anfang - Ende) einrichten</t>
+  </si>
+  <si>
+    <t>tixi_fahrzeug_details_page</t>
+  </si>
+  <si>
+    <t>/app/fahrzeug/details</t>
+  </si>
+  <si>
+    <t>Fahrzeug - Details</t>
+  </si>
+  <si>
+    <t>Vertrauliche Daten zur Fahrzeug</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1284,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1398,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f t="shared" ref="A4:A47" si="0">A3+1</f>
+        <f t="shared" ref="A4:A48" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2413,7 +2425,7 @@
         <v>169</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>118</v>
+        <v>231</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>117</v>
@@ -2422,19 +2434,19 @@
         <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>80</v>
+        <v>232</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>196</v>
+        <v>233</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>97</v>
+        <v>234</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2446,22 +2458,25 @@
         <v>169</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="E38" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>140</v>
+        <v>196</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>97</v>
@@ -2476,25 +2491,25 @@
         <v>169</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E39" s="12">
         <v>0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>141</v>
+        <v>10</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2506,22 +2521,22 @@
         <v>169</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>213</v>
+        <v>127</v>
       </c>
       <c r="E40" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>214</v>
+        <v>89</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>20</v>
+        <v>201</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>98</v>
@@ -2536,22 +2551,22 @@
         <v>169</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="E41" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>90</v>
+        <v>214</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>98</v>
@@ -2566,22 +2581,22 @@
         <v>169</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E42" s="12">
         <v>0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>223</v>
+        <v>202</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>98</v>
@@ -2596,22 +2611,22 @@
         <v>169</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E43" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>35</v>
+        <v>203</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>98</v>
@@ -2626,22 +2641,22 @@
         <v>169</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E44" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>98</v>
@@ -2656,22 +2671,22 @@
         <v>169</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E45" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>98</v>
@@ -2686,22 +2701,22 @@
         <v>169</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>226</v>
+        <v>132</v>
       </c>
       <c r="E46" s="12">
         <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>227</v>
+        <v>94</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>228</v>
+        <v>58</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>230</v>
+        <v>11</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>98</v>
@@ -2716,31 +2731,61 @@
         <v>169</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E47" s="12">
         <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>98</v>
       </c>
     </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E48" s="12">
+        <v>1</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="F1:I45"/>
+  <autoFilter ref="F1:I46"/>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E45">
+  <conditionalFormatting sqref="E2:E46">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2750,7 +2795,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
+  <conditionalFormatting sqref="E48">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2760,7 +2805,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E47">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added Bundle Tixi/App/DriverScheduleBundle and upgraded the jQuery datepicker for tasks. Open issue: the date-shift pairs are not yet persisted in the database. The database access needs to be migrated out of the FormBuilder.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2335,7 +2335,7 @@
         <v>111</v>
       </c>
       <c r="E34" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Added caps-lock test for login, added two prototype bundles for driver recurring tasks and agenda. Added istAktive to driver schedule. Open issues: two prototypes.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -11,7 +11,7 @@
     <sheet name="help" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$47</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="240">
   <si>
     <t xml:space="preserve">Vertrauliche Daten zu Fahrer </t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Abwesend, annuliert Dauerauftraege waehrend ein oder mehrere Tagen.</t>
-  </si>
-  <si>
-    <t>Geplante Einsaetze vom Fahrer, wiederholend jede Woche</t>
   </si>
   <si>
     <t>Geplante Einsaetze vom Fahrer in ein Monat</t>
@@ -216,9 +213,6 @@
     <t>Anrufmaske</t>
   </si>
   <si>
-    <t>Wochenplan</t>
-  </si>
-  <si>
     <t>Ferienplan</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
     <t>/app/fahrer</t>
   </si>
   <si>
-    <t>/app/fahrer/wochenplan</t>
-  </si>
-  <si>
     <t>/app/fahrer/ferienplan</t>
   </si>
   <si>
@@ -417,9 +408,6 @@
     <t>tixi_fahrer_page</t>
   </si>
   <si>
-    <t>tixi_fahrer_wochenplan_page</t>
-  </si>
-  <si>
     <t>tixi_fahrer_ferienplan_page</t>
   </si>
   <si>
@@ -654,9 +642,6 @@
     <t>Fahrgast - Anrufmaske</t>
   </si>
   <si>
-    <t>Fahrer - Wochenplan</t>
-  </si>
-  <si>
     <t>Fahrer - Ferienplan</t>
   </si>
   <si>
@@ -784,6 +769,36 @@
   </si>
   <si>
     <t>Vertrauliche Daten zur Fahrzeug</t>
+  </si>
+  <si>
+    <t>tixi_fahrer_dauereinsatz_page</t>
+  </si>
+  <si>
+    <t>/app/fahrer/dauereinsatz</t>
+  </si>
+  <si>
+    <t>Dauereinsatz</t>
+  </si>
+  <si>
+    <t>Geplante Einsaetze vom Fahrer, wiederholend wöchetlich, monatlich</t>
+  </si>
+  <si>
+    <t>Fahrer - Dauereinsatz</t>
+  </si>
+  <si>
+    <t>tixi_fahrer_agenda_page</t>
+  </si>
+  <si>
+    <t>/app/fahrer/agenda</t>
+  </si>
+  <si>
+    <t>Agenda</t>
+  </si>
+  <si>
+    <t>Fahrer - Agenda</t>
+  </si>
+  <si>
+    <t>Uebersicht aller Einsätze, Dauereinsätze, Ferien und Feiertage</t>
   </si>
 </sst>
 </file>
@@ -1284,10 +1299,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1307,19 +1322,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>12</v>
@@ -1328,7 +1343,7 @@
         <v>13</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>19</v>
@@ -1342,28 +1357,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1372,58 +1387,58 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f t="shared" ref="A4:A48" si="0">A3+1</f>
+        <f t="shared" ref="A4:A49" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1432,28 +1447,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1462,28 +1477,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E6" s="12">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1492,28 +1507,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E7" s="12">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1522,28 +1537,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E8" s="12">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1552,28 +1567,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E9" s="12">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1582,16 +1597,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E10" s="12">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>5</v>
@@ -1600,10 +1615,10 @@
         <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1612,28 +1627,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1642,28 +1657,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E12" s="12">
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1672,28 +1687,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E13" s="12">
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1702,28 +1717,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E14" s="12">
         <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1732,28 +1747,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E15" s="12">
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1762,16 +1777,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E16" s="12">
         <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>9</v>
@@ -1780,10 +1795,10 @@
         <v>9</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1792,28 +1807,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1822,28 +1837,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E18" s="12">
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1852,28 +1867,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E19" s="12">
         <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1882,28 +1897,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1912,28 +1927,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E21" s="12">
         <v>0</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1942,28 +1957,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E22" s="12">
         <v>0</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1972,16 +1987,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E23" s="12">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>18</v>
@@ -1990,10 +2005,10 @@
         <v>18</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2002,31 +2017,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E24" s="12">
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2035,31 +2050,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E25" s="12">
         <v>0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2068,31 +2083,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E26" s="12">
         <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2101,31 +2116,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E27" s="12">
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2134,16 +2149,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E28" s="12">
         <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>14</v>
@@ -2152,10 +2167,10 @@
         <v>14</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2164,31 +2179,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E29" s="12">
         <v>1</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2197,16 +2212,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E30" s="12">
         <v>1</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>15</v>
@@ -2215,10 +2230,10 @@
         <v>15</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2227,31 +2242,31 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E31" s="12">
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2260,31 +2275,31 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>230</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E32" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>74</v>
+        <v>231</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>45</v>
+        <v>232</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>26</v>
+        <v>233</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2293,31 +2308,31 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E33" s="12">
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2326,31 +2341,31 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E34" s="12">
         <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2359,31 +2374,31 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>116</v>
+        <v>235</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E35" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>78</v>
+        <v>236</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>44</v>
+        <v>237</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>195</v>
+        <v>238</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>1</v>
+        <v>239</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2392,28 +2407,31 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="E36" s="12">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="J36" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2422,31 +2440,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E37" s="12">
         <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>232</v>
+        <v>76</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>233</v>
+        <v>16</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>98</v>
+        <v>2</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2455,31 +2470,31 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>118</v>
+        <v>226</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E38" s="12">
         <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>80</v>
+        <v>227</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>97</v>
+        <v>229</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2488,28 +2503,31 @@
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="E39" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>140</v>
+        <v>191</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2518,28 +2536,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E40" s="12">
         <v>0</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>141</v>
+        <v>10</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2548,28 +2566,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
       <c r="E41" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>214</v>
+        <v>86</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>20</v>
+        <v>196</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2578,28 +2596,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>128</v>
+        <v>208</v>
       </c>
       <c r="E42" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>90</v>
+        <v>209</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2608,28 +2626,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E43" s="12">
         <v>0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>223</v>
+        <v>197</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2638,28 +2656,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E44" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>35</v>
+        <v>198</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2668,28 +2686,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E45" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2698,28 +2716,28 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E46" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2728,28 +2746,28 @@
         <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>226</v>
+        <v>128</v>
       </c>
       <c r="E47" s="12">
         <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>227</v>
+        <v>91</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>228</v>
+        <v>56</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>230</v>
+        <v>11</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2758,34 +2776,64 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E48" s="12">
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="12">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E49" s="12">
+        <v>1</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I46"/>
+  <autoFilter ref="F1:I47"/>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E46">
+  <conditionalFormatting sqref="E2:E47">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2795,7 +2843,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
+  <conditionalFormatting sqref="E49">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2805,7 +2853,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
+  <conditionalFormatting sqref="E48">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2841,7 +2889,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2852,7 +2900,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2863,7 +2911,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2874,7 +2922,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>

</xml_diff>

<commit_message>
Finished coding and testing Driver Agenda. Query logic embedded in database views agenda* (5 views). Upgraded backup with --routines option, and added backups to the git repository. Added menue option Fahrgast - Einzelauftrag, changed menu option Fahrer - Dauerauftrag to Dauerauftragplan. Added field fahrer_einsatzwunsch to table Fahrer. Open issue "Send email" to be implemented later, see SRS-List.
</commit_message>
<xml_diff>
--- a/web/doc/MenuTree.xlsx
+++ b/web/doc/MenuTree.xlsx
@@ -11,7 +11,7 @@
     <sheet name="help" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$I$48</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="245">
   <si>
     <t xml:space="preserve">Vertrauliche Daten zu Fahrer </t>
   </si>
@@ -771,21 +771,9 @@
     <t>Vertrauliche Daten zur Fahrzeug</t>
   </si>
   <si>
-    <t>tixi_fahrer_dauereinsatz_page</t>
-  </si>
-  <si>
-    <t>/app/fahrer/dauereinsatz</t>
-  </si>
-  <si>
-    <t>Dauereinsatz</t>
-  </si>
-  <si>
     <t>Geplante Einsaetze vom Fahrer, wiederholend wöchetlich, monatlich</t>
   </si>
   <si>
-    <t>Fahrer - Dauereinsatz</t>
-  </si>
-  <si>
     <t>tixi_fahrer_agenda_page</t>
   </si>
   <si>
@@ -799,6 +787,33 @@
   </si>
   <si>
     <t>Uebersicht aller Einsätze, Dauereinsätze, Ferien und Feiertage</t>
+  </si>
+  <si>
+    <t>Dauereinsatzplan</t>
+  </si>
+  <si>
+    <t>Fahrer - Dauereinsatzplan</t>
+  </si>
+  <si>
+    <t>/app/fahrer/dauereinsatzplan</t>
+  </si>
+  <si>
+    <t>tixi_fahrer_dauereinsatzplan_page</t>
+  </si>
+  <si>
+    <t>tixi_fahrgast_einzelauftrag_page</t>
+  </si>
+  <si>
+    <t>/app/fahrgast/einzelauftrag</t>
+  </si>
+  <si>
+    <t>Fahrgast - Einzelauftrag</t>
+  </si>
+  <si>
+    <t>Ein einzelne Fahrauftrag (einmalig, wiederholt nicht).</t>
+  </si>
+  <si>
+    <t>Einzelauftrag</t>
   </si>
 </sst>
 </file>
@@ -1299,10 +1314,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1428,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f t="shared" ref="A4:A49" si="0">A3+1</f>
+        <f t="shared" ref="A4:A50" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2044,7 +2059,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2053,7 +2068,7 @@
         <v>165</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>103</v>
+        <v>240</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>102</v>
@@ -2062,22 +2077,22 @@
         <v>0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>40</v>
+        <v>244</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>183</v>
+        <v>242</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>24</v>
+        <v>243</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2086,25 +2101,25 @@
         <v>165</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E26" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>94</v>
@@ -2119,25 +2134,25 @@
         <v>165</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E27" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>94</v>
@@ -2152,22 +2167,25 @@
         <v>165</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="E28" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>212</v>
+        <v>43</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>94</v>
@@ -2182,28 +2200,25 @@
         <v>165</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" s="1" t="s">
         <v>107</v>
       </c>
       <c r="E29" s="12">
         <v>1</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>206</v>
+      <c r="F29" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>207</v>
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2215,25 +2230,28 @@
         <v>165</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>108</v>
+        <v>205</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="E30" s="12">
         <v>1</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>71</v>
+        <v>206</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>213</v>
+        <v>42</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2245,28 +2263,25 @@
         <v>165</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="1" t="s">
         <v>108</v>
       </c>
       <c r="E31" s="12">
         <v>1</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>74</v>
+      <c r="F31" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2278,7 +2293,7 @@
         <v>165</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>230</v>
+        <v>111</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>108</v>
@@ -2287,19 +2302,19 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>231</v>
+        <v>74</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>232</v>
+        <v>42</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>234</v>
+        <v>189</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>233</v>
+        <v>0</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2311,7 +2326,7 @@
         <v>165</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>109</v>
+        <v>239</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>108</v>
@@ -2320,16 +2335,16 @@
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>72</v>
+        <v>238</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>44</v>
+        <v>236</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>32</v>
+        <v>230</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>94</v>
@@ -2344,7 +2359,7 @@
         <v>165</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>108</v>
@@ -2353,16 +2368,16 @@
         <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>94</v>
@@ -2377,7 +2392,7 @@
         <v>165</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>235</v>
+        <v>110</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>108</v>
@@ -2386,16 +2401,16 @@
         <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>236</v>
+        <v>73</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>237</v>
+        <v>45</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>239</v>
+        <v>26</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>94</v>
@@ -2410,25 +2425,25 @@
         <v>165</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>112</v>
+        <v>231</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>108</v>
       </c>
       <c r="E36" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>75</v>
+        <v>232</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>43</v>
+        <v>233</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>1</v>
+        <v>235</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>94</v>
@@ -2443,22 +2458,25 @@
         <v>165</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="E37" s="12">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>94</v>
@@ -2473,28 +2491,25 @@
         <v>165</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D38" s="1" t="s">
         <v>113</v>
       </c>
       <c r="E38" s="12">
         <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>227</v>
+        <v>76</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>228</v>
+        <v>16</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>95</v>
+        <v>2</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2506,7 +2521,7 @@
         <v>165</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>226</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>113</v>
@@ -2515,19 +2530,19 @@
         <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>77</v>
+        <v>227</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>94</v>
+        <v>229</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2539,22 +2554,25 @@
         <v>165</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="E40" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>136</v>
+        <v>191</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>94</v>
@@ -2569,25 +2587,25 @@
         <v>165</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E41" s="12">
         <v>0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>137</v>
+        <v>10</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2599,22 +2617,22 @@
         <v>165</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="E42" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>209</v>
+        <v>86</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>20</v>
+        <v>196</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>95</v>
@@ -2629,22 +2647,22 @@
         <v>165</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="E43" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>87</v>
+        <v>209</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>95</v>
@@ -2659,22 +2677,22 @@
         <v>165</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E44" s="12">
         <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>218</v>
+        <v>197</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>95</v>
@@ -2689,22 +2707,22 @@
         <v>165</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E45" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>34</v>
+        <v>198</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>95</v>
@@ -2719,22 +2737,22 @@
         <v>165</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E46" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>95</v>
@@ -2749,22 +2767,22 @@
         <v>165</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E47" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>95</v>
@@ -2779,22 +2797,22 @@
         <v>165</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>221</v>
+        <v>128</v>
       </c>
       <c r="E48" s="12">
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>222</v>
+        <v>91</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>223</v>
+        <v>56</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>225</v>
+        <v>11</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>95</v>
@@ -2809,31 +2827,61 @@
         <v>165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E49" s="12">
         <v>1</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>95</v>
       </c>
     </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E50" s="12">
+        <v>1</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="F1:I47"/>
+  <autoFilter ref="F1:I48"/>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E47">
+  <conditionalFormatting sqref="E2:E48">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2843,7 +2891,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
+  <conditionalFormatting sqref="E50">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2853,7 +2901,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
+  <conditionalFormatting sqref="E49">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>